<commit_message>
this model is ps1,ps6 only ,0.8~1.5 , deaklock
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum Yes ob pipe_section 0_1/Curriculum Yes ob pipe_section 0_1_test_pipe_section_2/Curriculum Yes ob pipe_section 0_1_test_pipe_section_2_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum Yes ob pipe_section 0_1/Curriculum Yes ob pipe_section 0_1_test_pipe_section_2/Curriculum Yes ob pipe_section 0_1_test_pipe_section_2_Test_Result.xlsx
@@ -445,16 +445,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
model 8 reward best ok.
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum Yes ob pipe_section 0_1/Curriculum Yes ob pipe_section 0_1_test_pipe_section_2/Curriculum Yes ob pipe_section 0_1_test_pipe_section_2_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum Yes ob pipe_section 0_1/Curriculum Yes ob pipe_section 0_1_test_pipe_section_2/Curriculum Yes ob pipe_section 0_1_test_pipe_section_2_Test_Result.xlsx
@@ -445,16 +445,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.975</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reward 직진 ++ -> the best
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum Yes ob pipe_section 0_1/Curriculum Yes ob pipe_section 0_1_test_pipe_section_2/Curriculum Yes ob pipe_section 0_1_test_pipe_section_2_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum Yes ob pipe_section 0_1/Curriculum Yes ob pipe_section 0_1_test_pipe_section_2/Curriculum Yes ob pipe_section 0_1_test_pipe_section_2_Test_Result.xlsx
@@ -448,13 +448,13 @@
         <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.975</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>